<commit_message>
actualizacion de vistas de formularios en general
</commit_message>
<xml_diff>
--- a/Files/Temp_inv/1.xlsx
+++ b/Files/Temp_inv/1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TECNOLOGIA-LOGI\Documents\LOGI\Carga Masiva\Masivo Inventario Alistamiento\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7485"/>
   </bookViews>
@@ -1661,9 +1656,6 @@
     <t>064CS24872</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>605CS25799</t>
   </si>
   <si>
@@ -1923,12 +1915,15 @@
   </si>
   <si>
     <t>6A</t>
+  </si>
+  <si>
+    <t>SERT0002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -2116,7 +2111,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2151,7 +2146,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2362,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="B234" sqref="B234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2427,7 +2422,7 @@
         <v>42</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F3">
         <v>30000</v>
@@ -2507,7 +2502,7 @@
         <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F7">
         <v>40000</v>
@@ -2524,7 +2519,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>242</v>
@@ -2544,7 +2539,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>242</v>
@@ -2607,7 +2602,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F12">
         <v>50000</v>
@@ -2647,7 +2642,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F14">
         <v>40000</v>
@@ -2664,10 +2659,10 @@
         <v>38</v>
       </c>
       <c r="D15" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F15">
         <v>50000</v>
@@ -2704,7 +2699,7 @@
         <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>247</v>
@@ -2724,10 +2719,10 @@
         <v>44</v>
       </c>
       <c r="D18" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F18">
         <v>50000</v>
@@ -2744,7 +2739,7 @@
         <v>46</v>
       </c>
       <c r="D19" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>239</v>
@@ -2764,7 +2759,7 @@
         <v>48</v>
       </c>
       <c r="D20" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>244</v>
@@ -2804,7 +2799,7 @@
         <v>52</v>
       </c>
       <c r="D22" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>244</v>
@@ -2864,7 +2859,7 @@
         <v>56</v>
       </c>
       <c r="D25" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>248</v>
@@ -2907,7 +2902,7 @@
         <v>44</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F27">
         <v>50000</v>
@@ -2947,7 +2942,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F29">
         <v>50000</v>
@@ -2987,7 +2982,7 @@
         <v>25</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F31">
         <v>50000</v>
@@ -3027,7 +3022,7 @@
         <v>16</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F33">
         <v>50000</v>
@@ -3064,7 +3059,7 @@
         <v>75</v>
       </c>
       <c r="D35" s="2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>247</v>
@@ -3087,7 +3082,7 @@
         <v>37</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F36">
         <v>50000</v>
@@ -3147,7 +3142,7 @@
         <v>44</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F39">
         <v>50000</v>
@@ -3167,7 +3162,7 @@
         <v>35</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F40">
         <v>40000</v>
@@ -3187,7 +3182,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F41">
         <v>50000</v>
@@ -3207,7 +3202,7 @@
         <v>40</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F42">
         <v>50000</v>
@@ -3224,10 +3219,10 @@
         <v>91</v>
       </c>
       <c r="D43" s="2">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F43">
         <v>50000</v>
@@ -3264,7 +3259,7 @@
         <v>95</v>
       </c>
       <c r="D45" s="2">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>242</v>
@@ -3284,7 +3279,7 @@
         <v>97</v>
       </c>
       <c r="D46" s="2">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>247</v>
@@ -3304,10 +3299,10 @@
         <v>99</v>
       </c>
       <c r="D47" s="2">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F47">
         <v>50000</v>
@@ -3327,7 +3322,7 @@
         <v>50</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F48">
         <v>40000</v>
@@ -3344,7 +3339,7 @@
         <v>103</v>
       </c>
       <c r="D49" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>244</v>
@@ -3367,7 +3362,7 @@
         <v>19</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F50">
         <v>40000</v>
@@ -3404,10 +3399,10 @@
         <v>109</v>
       </c>
       <c r="D52" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F52">
         <v>40000</v>
@@ -3447,7 +3442,7 @@
         <v>25</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F54">
         <v>50000</v>
@@ -3467,7 +3462,7 @@
         <v>30</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F55">
         <v>50000</v>
@@ -3507,7 +3502,7 @@
         <v>50</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F57">
         <v>40000</v>
@@ -3524,10 +3519,10 @@
         <v>121</v>
       </c>
       <c r="D58" s="2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F58">
         <v>50000</v>
@@ -3547,7 +3542,7 @@
         <v>25</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F59">
         <v>30000</v>
@@ -3567,7 +3562,7 @@
         <v>20</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F60">
         <v>30000</v>
@@ -3604,7 +3599,7 @@
         <v>129</v>
       </c>
       <c r="D62" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>249</v>
@@ -3684,7 +3679,7 @@
         <v>137</v>
       </c>
       <c r="D66" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>249</v>
@@ -3727,7 +3722,7 @@
         <v>17</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F68">
         <v>50000</v>
@@ -3787,7 +3782,7 @@
         <v>50</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F71">
         <v>50000</v>
@@ -3827,7 +3822,7 @@
         <v>29</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F73">
         <v>40000</v>
@@ -3867,7 +3862,7 @@
         <v>28</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F75">
         <v>40000</v>
@@ -3904,10 +3899,10 @@
         <v>159</v>
       </c>
       <c r="D77" s="2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F77">
         <v>30000</v>
@@ -3927,7 +3922,7 @@
         <v>12</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F78">
         <v>30000</v>
@@ -3947,7 +3942,7 @@
         <v>38</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F79">
         <v>50000</v>
@@ -4044,7 +4039,7 @@
         <v>173</v>
       </c>
       <c r="D84" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>244</v>
@@ -4064,10 +4059,10 @@
         <v>175</v>
       </c>
       <c r="D85" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F85">
         <v>50000</v>
@@ -4087,7 +4082,7 @@
         <v>25</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F86">
         <v>40000</v>
@@ -4107,7 +4102,7 @@
         <v>40</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F87">
         <v>50000</v>
@@ -4124,10 +4119,10 @@
         <v>181</v>
       </c>
       <c r="D88" s="2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F88">
         <v>40000</v>
@@ -4144,10 +4139,10 @@
         <v>183</v>
       </c>
       <c r="D89" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F89">
         <v>50000</v>
@@ -4164,10 +4159,10 @@
         <v>185</v>
       </c>
       <c r="D90" s="2">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F90">
         <v>50000</v>
@@ -4187,7 +4182,7 @@
         <v>25</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F91">
         <v>50000</v>
@@ -4227,7 +4222,7 @@
         <v>20</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F93">
         <v>40000</v>
@@ -4284,7 +4279,7 @@
         <v>196</v>
       </c>
       <c r="D96" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>251</v>
@@ -4327,7 +4322,7 @@
         <v>15</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F98">
         <v>40000</v>
@@ -4407,7 +4402,7 @@
         <v>15</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F102">
         <v>50000</v>
@@ -4424,7 +4419,7 @@
         <v>210</v>
       </c>
       <c r="D103" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>245</v>
@@ -4507,7 +4502,7 @@
         <v>21</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F107">
         <v>30000</v>
@@ -4547,7 +4542,7 @@
         <v>25</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F109">
         <v>50000</v>
@@ -4564,10 +4559,10 @@
         <v>224</v>
       </c>
       <c r="D110" s="2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F110">
         <v>40000</v>
@@ -4647,7 +4642,7 @@
         <v>16</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F114">
         <v>30000</v>
@@ -4664,10 +4659,10 @@
         <v>232</v>
       </c>
       <c r="D115" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F115">
         <v>50000</v>
@@ -4707,7 +4702,7 @@
         <v>19</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F117">
         <v>40000</v>
@@ -4787,7 +4782,7 @@
         <v>10</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F121">
         <v>50000</v>
@@ -4807,7 +4802,7 @@
         <v>10</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F122">
         <v>40000</v>
@@ -4827,7 +4822,7 @@
         <v>10</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F123">
         <v>50000</v>
@@ -4847,7 +4842,7 @@
         <v>10</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F124">
         <v>50000</v>
@@ -4867,7 +4862,7 @@
         <v>25</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F125">
         <v>40000</v>
@@ -4884,10 +4879,10 @@
         <v>267</v>
       </c>
       <c r="D126" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F126">
         <v>50000</v>
@@ -4907,7 +4902,7 @@
         <v>12</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F127">
         <v>50000</v>
@@ -4967,7 +4962,7 @@
         <v>25</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F130">
         <v>40000</v>
@@ -4987,7 +4982,7 @@
         <v>16</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F131">
         <v>50000</v>
@@ -5007,7 +5002,7 @@
         <v>15</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F132">
         <v>50000</v>
@@ -5047,7 +5042,7 @@
         <v>10</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F134">
         <v>50000</v>
@@ -5067,7 +5062,7 @@
         <v>20</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F135">
         <v>40000</v>
@@ -5124,7 +5119,7 @@
         <v>279</v>
       </c>
       <c r="D138" s="2">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>240</v>
@@ -5147,7 +5142,7 @@
         <v>21</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F139">
         <v>50000</v>
@@ -5167,7 +5162,7 @@
         <v>19</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F140">
         <v>40000</v>
@@ -5207,7 +5202,7 @@
         <v>18</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F142">
         <v>50000</v>
@@ -5227,7 +5222,7 @@
         <v>17</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F143">
         <v>30000</v>
@@ -5287,7 +5282,7 @@
         <v>30</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F146">
         <v>50000</v>
@@ -5307,7 +5302,7 @@
         <v>32</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F147">
         <v>40000</v>
@@ -5327,7 +5322,7 @@
         <v>26</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F148">
         <v>50000</v>
@@ -5347,7 +5342,7 @@
         <v>22</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F149">
         <v>50000</v>
@@ -5367,7 +5362,7 @@
         <v>20</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F150">
         <v>50000</v>
@@ -5387,7 +5382,7 @@
         <v>13</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F151">
         <v>50000</v>
@@ -5407,7 +5402,7 @@
         <v>15</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F152">
         <v>40000</v>
@@ -5427,7 +5422,7 @@
         <v>12</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F153">
         <v>50000</v>
@@ -5444,7 +5439,7 @@
         <v>295</v>
       </c>
       <c r="D154" s="2">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>248</v>
@@ -5464,10 +5459,10 @@
         <v>296</v>
       </c>
       <c r="D155" s="2">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F155">
         <v>40000</v>
@@ -5504,7 +5499,7 @@
         <v>298</v>
       </c>
       <c r="D157" s="2">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E157" s="3" t="s">
         <v>247</v>
@@ -5644,10 +5639,10 @@
         <v>305</v>
       </c>
       <c r="D164" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F164">
         <v>50000</v>
@@ -5664,7 +5659,7 @@
         <v>306</v>
       </c>
       <c r="D165" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>242</v>
@@ -5684,7 +5679,7 @@
         <v>307</v>
       </c>
       <c r="D166" s="2">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>9</v>
@@ -5704,7 +5699,7 @@
         <v>308</v>
       </c>
       <c r="D167" s="2">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>6</v>
@@ -5727,7 +5722,7 @@
         <v>20</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F168">
         <v>50000</v>
@@ -5747,7 +5742,7 @@
         <v>16</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F169">
         <v>40000</v>
@@ -5767,7 +5762,7 @@
         <v>40</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F170">
         <v>50000</v>
@@ -5827,7 +5822,7 @@
         <v>18</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F173">
         <v>50000</v>
@@ -5844,10 +5839,10 @@
         <v>315</v>
       </c>
       <c r="D174" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F174">
         <v>40000</v>
@@ -5867,7 +5862,7 @@
         <v>50</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F175">
         <v>50000</v>
@@ -5907,7 +5902,7 @@
         <v>20</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F177">
         <v>40000</v>
@@ -5967,7 +5962,7 @@
         <v>25</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F180">
         <v>50000</v>
@@ -5987,7 +5982,7 @@
         <v>20</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F181">
         <v>50000</v>
@@ -6044,10 +6039,10 @@
         <v>325</v>
       </c>
       <c r="D184" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F184">
         <v>40000</v>
@@ -6087,7 +6082,7 @@
         <v>19</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F186">
         <v>50000</v>
@@ -6107,7 +6102,7 @@
         <v>15</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F187">
         <v>30000</v>
@@ -6144,7 +6139,7 @@
         <v>330</v>
       </c>
       <c r="D189" s="2">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>251</v>
@@ -6164,7 +6159,7 @@
         <v>331</v>
       </c>
       <c r="D190" s="2">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E190" s="3" t="s">
         <v>252</v>
@@ -6187,7 +6182,7 @@
         <v>15</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F191">
         <v>40000</v>
@@ -6204,10 +6199,10 @@
         <v>333</v>
       </c>
       <c r="D192" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F192">
         <v>50000</v>
@@ -6227,7 +6222,7 @@
         <v>10</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F193">
         <v>50000</v>
@@ -6247,7 +6242,7 @@
         <v>20</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F194">
         <v>50000</v>
@@ -6267,7 +6262,7 @@
         <v>20</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F195">
         <v>50000</v>
@@ -6287,7 +6282,7 @@
         <v>25</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F196">
         <v>40000</v>
@@ -6307,7 +6302,7 @@
         <v>10</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F197">
         <v>50000</v>
@@ -6327,7 +6322,7 @@
         <v>30</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F198">
         <v>50000</v>
@@ -6344,10 +6339,10 @@
         <v>340</v>
       </c>
       <c r="D199" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E199" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F199">
         <v>40000</v>
@@ -6364,7 +6359,7 @@
         <v>341</v>
       </c>
       <c r="D200" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>247</v>
@@ -6384,7 +6379,7 @@
         <v>342</v>
       </c>
       <c r="D201" s="2">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>243</v>
@@ -6404,7 +6399,7 @@
         <v>343</v>
       </c>
       <c r="D202" s="2">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>11</v>
@@ -6447,7 +6442,7 @@
         <v>16</v>
       </c>
       <c r="E204" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F204">
         <v>50000</v>
@@ -6467,7 +6462,7 @@
         <v>40</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F205">
         <v>50000</v>
@@ -6547,7 +6542,7 @@
         <v>10</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F209">
         <v>30000</v>
@@ -6604,7 +6599,7 @@
         <v>353</v>
       </c>
       <c r="D212" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>9</v>
@@ -6624,7 +6619,7 @@
         <v>354</v>
       </c>
       <c r="D213" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>244</v>
@@ -6647,7 +6642,7 @@
         <v>25</v>
       </c>
       <c r="E214" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F214">
         <v>50000</v>
@@ -6687,7 +6682,7 @@
         <v>23</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F216">
         <v>50000</v>
@@ -6744,7 +6739,7 @@
         <v>360</v>
       </c>
       <c r="D219" s="2">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>243</v>
@@ -6784,10 +6779,10 @@
         <v>362</v>
       </c>
       <c r="D221" s="2">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F221">
         <v>40000</v>
@@ -6804,7 +6799,7 @@
         <v>363</v>
       </c>
       <c r="D222" s="2">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>242</v>
@@ -6824,7 +6819,7 @@
         <v>364</v>
       </c>
       <c r="D223" s="2">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>246</v>
@@ -6844,7 +6839,7 @@
         <v>365</v>
       </c>
       <c r="D224" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>244</v>
@@ -6867,7 +6862,7 @@
         <v>10</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F225">
         <v>50000</v>
@@ -6884,10 +6879,10 @@
         <v>367</v>
       </c>
       <c r="D226" s="2">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F226">
         <v>50000</v>
@@ -6907,7 +6902,7 @@
         <v>30</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F227">
         <v>50000</v>
@@ -6927,7 +6922,7 @@
         <v>18</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F228">
         <v>40000</v>
@@ -6944,10 +6939,10 @@
         <v>370</v>
       </c>
       <c r="D229" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F229">
         <v>50000</v>
@@ -6987,7 +6982,7 @@
         <v>30</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F231">
         <v>30000</v>
@@ -7004,7 +6999,7 @@
         <v>373</v>
       </c>
       <c r="D232" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>246</v>
@@ -7018,7 +7013,7 @@
         <v>8809582396172</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>545</v>
+        <v>632</v>
       </c>
       <c r="C233" s="3" t="s">
         <v>374</v>
@@ -7027,7 +7022,7 @@
         <v>37</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F233">
         <v>50000</v>
@@ -7038,7 +7033,7 @@
         <v>8809640252266</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C234" s="3" t="s">
         <v>375</v>
@@ -7047,7 +7042,7 @@
         <v>19</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F234">
         <v>50000</v>
@@ -7058,7 +7053,7 @@
         <v>8809466648939</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C235" s="3" t="s">
         <v>376</v>
@@ -7067,7 +7062,7 @@
         <v>15</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F235">
         <v>40000</v>
@@ -7078,7 +7073,7 @@
         <v>8809522196299</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C236" s="3" t="s">
         <v>377</v>
@@ -7098,7 +7093,7 @@
         <v>8808522199474</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C237" s="3" t="s">
         <v>378</v>
@@ -7118,7 +7113,7 @@
         <v>8809522191454</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C238" s="3" t="s">
         <v>379</v>
@@ -7138,7 +7133,7 @@
         <v>8809640259739</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C239" s="3" t="s">
         <v>380</v>
@@ -7147,7 +7142,7 @@
         <v>10</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F239">
         <v>50000</v>
@@ -7158,7 +7153,7 @@
         <v>8809565303371</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>381</v>
@@ -7167,7 +7162,7 @@
         <v>40</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F240">
         <v>40000</v>
@@ -7178,13 +7173,13 @@
         <v>8809466646270</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C241" s="3" t="s">
         <v>382</v>
       </c>
       <c r="D241" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>12</v>
@@ -7198,13 +7193,13 @@
         <v>8809466645396</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>383</v>
       </c>
       <c r="D242" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>7</v>
@@ -7218,7 +7213,7 @@
         <v>8809685622932</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C243" s="3" t="s">
         <v>384</v>
@@ -7238,7 +7233,7 @@
         <v>8809685625001</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C244" s="3" t="s">
         <v>385</v>
@@ -7258,7 +7253,7 @@
         <v>8809613766202</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C245" s="3" t="s">
         <v>386</v>
@@ -7278,7 +7273,7 @@
         <v>8809659043152</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C246" s="3" t="s">
         <v>387</v>
@@ -7287,7 +7282,7 @@
         <v>18</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F246">
         <v>50000</v>
@@ -7298,7 +7293,7 @@
         <v>8809659047747</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C247" s="3" t="s">
         <v>388</v>
@@ -7307,7 +7302,7 @@
         <v>30</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F247">
         <v>50000</v>
@@ -7318,13 +7313,13 @@
         <v>8809716075096</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C248" s="3" t="s">
         <v>389</v>
       </c>
       <c r="D248" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E248" s="3" t="s">
         <v>5</v>
@@ -7338,7 +7333,7 @@
         <v>8809659048638</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>390</v>
@@ -7358,16 +7353,16 @@
         <v>8809583842364</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C250" s="3" t="s">
         <v>391</v>
       </c>
       <c r="D250" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E250" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F250">
         <v>40000</v>
@@ -7378,16 +7373,16 @@
         <v>8809716075669</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C251" s="3" t="s">
         <v>392</v>
       </c>
       <c r="D251" s="2">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E251" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F251">
         <v>50000</v>
@@ -7398,16 +7393,16 @@
         <v>8809716075690</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C252" s="3" t="s">
         <v>393</v>
       </c>
       <c r="D252" s="2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F252">
         <v>50000</v>
@@ -7418,13 +7413,13 @@
         <v>8809716075720</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C253" s="3" t="s">
         <v>394</v>
       </c>
       <c r="D253" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E253" s="3" t="s">
         <v>253</v>
@@ -7435,10 +7430,10 @@
     </row>
     <row r="254" spans="1:6" ht="15.75" thickBot="1">
       <c r="A254" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C254" s="3" t="s">
         <v>395</v>
@@ -7455,16 +7450,16 @@
     </row>
     <row r="255" spans="1:6" ht="15.75" thickBot="1">
       <c r="A255" s="14" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B255" s="14" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>396</v>
       </c>
       <c r="D255" s="2">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E255" s="3" t="s">
         <v>245</v>
@@ -7475,10 +7470,10 @@
     </row>
     <row r="256" spans="1:6" ht="15.75" thickBot="1">
       <c r="A256" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>397</v>
@@ -7487,7 +7482,7 @@
         <v>30</v>
       </c>
       <c r="E256" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F256">
         <v>50000</v>
@@ -7495,10 +7490,10 @@
     </row>
     <row r="257" spans="1:6" ht="15.75" thickBot="1">
       <c r="A257" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>398</v>
@@ -7515,16 +7510,16 @@
     </row>
     <row r="258" spans="1:6" ht="15.75" thickBot="1">
       <c r="A258" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C258" s="3" t="s">
         <v>399</v>
       </c>
       <c r="D258" s="2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E258" s="3" t="s">
         <v>247</v>
@@ -7535,10 +7530,10 @@
     </row>
     <row r="259" spans="1:6" ht="15.75" thickBot="1">
       <c r="A259" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>400</v>
@@ -7547,7 +7542,7 @@
         <v>50</v>
       </c>
       <c r="E259" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F259">
         <v>50000</v>
@@ -7555,10 +7550,10 @@
     </row>
     <row r="260" spans="1:6" ht="15.75" thickBot="1">
       <c r="A260" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>401</v>
@@ -7578,7 +7573,7 @@
         <v>8809613760361</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C261" s="3" t="s">
         <v>402</v>
@@ -7587,7 +7582,7 @@
         <v>30</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F261">
         <v>50000</v>
@@ -7598,16 +7593,16 @@
         <v>8809685626558</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C262" s="3" t="s">
         <v>403</v>
       </c>
       <c r="D262" s="2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F262">
         <v>40000</v>
@@ -7618,7 +7613,7 @@
         <v>8809685626176</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>404</v>
@@ -7627,7 +7622,7 @@
         <v>37</v>
       </c>
       <c r="E263" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F263">
         <v>50000</v>
@@ -7638,7 +7633,7 @@
         <v>8809640258718</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>405</v>
@@ -7647,7 +7642,7 @@
         <v>19</v>
       </c>
       <c r="E264" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F264">
         <v>50000</v>
@@ -7658,7 +7653,7 @@
         <v>8809671010248</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>406</v>
@@ -7667,7 +7662,7 @@
         <v>15</v>
       </c>
       <c r="E265" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F265">
         <v>40000</v>
@@ -7678,7 +7673,7 @@
         <v>8809685624660</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>407</v>
@@ -7687,7 +7682,7 @@
         <v>42</v>
       </c>
       <c r="E266" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F266">
         <v>50000</v>
@@ -7698,7 +7693,7 @@
         <v>8809685624042</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>408</v>
@@ -7707,7 +7702,7 @@
         <v>16</v>
       </c>
       <c r="E267" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F267">
         <v>40000</v>
@@ -7718,7 +7713,7 @@
         <v>8809565300202</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>409</v>
@@ -7727,7 +7722,7 @@
         <v>10</v>
       </c>
       <c r="E268" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F268">
         <v>50000</v>
@@ -7738,7 +7733,7 @@
         <v>8809671010293</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C269" s="3" t="s">
         <v>410</v>
@@ -7747,7 +7742,7 @@
         <v>10</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F269">
         <v>50000</v>
@@ -7758,7 +7753,7 @@
         <v>8809716075751</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C270" s="3" t="s">
         <v>411</v>
@@ -7767,7 +7762,7 @@
         <v>40</v>
       </c>
       <c r="E270" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F270">
         <v>50000</v>
@@ -7778,13 +7773,13 @@
         <v>8809685623991</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>412</v>
       </c>
       <c r="D271" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E271" s="3" t="s">
         <v>9</v>
@@ -7798,16 +7793,16 @@
         <v>8809685627081</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>413</v>
       </c>
       <c r="D272" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E272" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F272">
         <v>40000</v>
@@ -7815,10 +7810,10 @@
     </row>
     <row r="273" spans="1:6" ht="15.75" thickBot="1">
       <c r="A273" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>414</v>
@@ -7827,7 +7822,7 @@
         <v>25</v>
       </c>
       <c r="E273" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F273">
         <v>50000</v>
@@ -7838,7 +7833,7 @@
         <v>8809685625469</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>415</v>
@@ -7847,7 +7842,7 @@
         <v>25</v>
       </c>
       <c r="E274" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F274">
         <v>50000</v>
@@ -7858,7 +7853,7 @@
         <v>8809640250392</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>416</v>
@@ -7867,7 +7862,7 @@
         <v>23</v>
       </c>
       <c r="E275" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F275">
         <v>30000</v>
@@ -7878,7 +7873,7 @@
         <v>8809685624035</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>417</v>
@@ -7898,7 +7893,7 @@
         <v>8809640251320</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C277" s="3" t="s">
         <v>418</v>
@@ -7918,13 +7913,13 @@
         <v>8809710751002</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C278" s="3" t="s">
         <v>419</v>
       </c>
       <c r="D278" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E278" s="3" t="s">
         <v>5</v>
@@ -7938,16 +7933,16 @@
         <v>8809685629344</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C279" s="3" t="s">
         <v>420</v>
       </c>
       <c r="D279" s="2">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E279" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F279">
         <v>50000</v>
@@ -7958,16 +7953,16 @@
         <v>8809565300950</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C280" s="3" t="s">
         <v>421</v>
       </c>
       <c r="D280" s="2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E280" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F280">
         <v>50000</v>
@@ -7975,16 +7970,16 @@
     </row>
     <row r="281" spans="1:6" ht="15.75" thickBot="1">
       <c r="A281" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C281" s="3" t="s">
         <v>422</v>
       </c>
       <c r="D281" s="2">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E281" s="3" t="s">
         <v>253</v>
@@ -7998,13 +7993,13 @@
         <v>8809716072446</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C282" s="3" t="s">
         <v>423</v>
       </c>
       <c r="D282" s="2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="E282" s="3" t="s">
         <v>11</v>
@@ -8018,16 +8013,16 @@
         <v>8809716072477</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>424</v>
       </c>
       <c r="D283" s="2">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E283" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F283">
         <v>40000</v>
@@ -8038,7 +8033,7 @@
         <v>8809716072507</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>425</v>
@@ -8047,7 +8042,7 @@
         <v>10</v>
       </c>
       <c r="E284" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F284">
         <v>50000</v>
@@ -8058,13 +8053,13 @@
         <v>8809716072538</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>426</v>
       </c>
       <c r="D285" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E285" s="3" t="s">
         <v>243</v>
@@ -8078,7 +8073,7 @@
         <v>8809716075577</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>427</v>
@@ -8098,7 +8093,7 @@
         <v>8809716075591</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C287" s="3" t="s">
         <v>428</v>
@@ -8118,16 +8113,16 @@
         <v>887276435336</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C288" s="3" t="s">
         <v>429</v>
       </c>
       <c r="D288" s="2">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E288" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F288">
         <v>50000</v>
@@ -8138,7 +8133,7 @@
         <v>887276435558</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C289" s="3" t="s">
         <v>430</v>
@@ -8147,7 +8142,7 @@
         <v>50</v>
       </c>
       <c r="E289" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F289">
         <v>50000</v>

</xml_diff>